<commit_message>
one more temp plot
</commit_message>
<xml_diff>
--- a/Data/HOBO-Data/Excel-Format/Compiled-Cross-Calibration-pre-pH.xlsx
+++ b/Data/HOBO-Data/Excel-Format/Compiled-Cross-Calibration-pre-pH.xlsx
@@ -197,8 +197,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -277,11 +277,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -323,6 +323,39 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>HOBO Temperature</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Cross Calibration, pre pH Trial</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>from 7pm -&gt; 1pm </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -3180,11 +3213,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2131624904"/>
-        <c:axId val="-2011883000"/>
+        <c:axId val="-1994813752"/>
+        <c:axId val="1785488200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2131624904"/>
+        <c:axId val="-1994813752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3218,12 +3251,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2011883000"/>
+        <c:crossAx val="1785488200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2011883000"/>
+        <c:axId val="1785488200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3253,7 +3286,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2131624904"/>
+        <c:crossAx val="-1994813752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3300,7 +3333,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>HOBO</a:t>
+              <a:t>HOBO Temp Residuals,</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -6241,11 +6274,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2074727432"/>
-        <c:axId val="-2075105160"/>
+        <c:axId val="-2078442104"/>
+        <c:axId val="-2078594024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2074727432"/>
+        <c:axId val="-2078442104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6281,12 +6314,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2075105160"/>
+        <c:crossAx val="-2078594024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2075105160"/>
+        <c:axId val="-2078594024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6320,7 +6353,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074727432"/>
+        <c:crossAx val="-2078442104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6733,8 +6766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B52" workbookViewId="0">
-      <selection activeCell="O76" sqref="O76"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AA12" sqref="AA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6812,7 +6845,7 @@
         <v>23.773</v>
       </c>
       <c r="H2" s="3">
-        <f>AVERAGE(B2:G2)</f>
+        <f t="shared" ref="H2:H33" si="0">AVERAGE(B2:G2)</f>
         <v>23.709</v>
       </c>
       <c r="I2" s="3">
@@ -6863,31 +6896,31 @@
         <v>23.581</v>
       </c>
       <c r="H3" s="3">
-        <f>AVERAGE(B3:G3)</f>
+        <f t="shared" si="0"/>
         <v>23.500499999999999</v>
       </c>
       <c r="I3" s="3">
-        <f t="shared" ref="I3:I66" si="0">H3-B3</f>
+        <f t="shared" ref="I3:I66" si="1">H3-B3</f>
         <v>-8.0500000000000682E-2</v>
       </c>
       <c r="J3" s="3">
-        <f t="shared" ref="J3:J66" si="1">H3-C3</f>
+        <f t="shared" ref="J3:J66" si="2">H3-C3</f>
         <v>-8.0500000000000682E-2</v>
       </c>
       <c r="K3" s="3">
-        <f t="shared" ref="K3:K17" si="2">$H3-D3</f>
+        <f t="shared" ref="K3:K16" si="3">$H3-D3</f>
         <v>1.6499999999997073E-2</v>
       </c>
       <c r="L3" s="3">
-        <f t="shared" ref="L3:L17" si="3">$H3-E3</f>
+        <f t="shared" ref="L3:L17" si="4">$H3-E3</f>
         <v>0.20849999999999724</v>
       </c>
       <c r="M3" s="3">
-        <f t="shared" ref="M3:M17" si="4">$H3-F3</f>
+        <f t="shared" ref="M3:M17" si="5">$H3-F3</f>
         <v>1.6499999999997073E-2</v>
       </c>
       <c r="N3" s="3">
-        <f t="shared" ref="N3:N17" si="5">$H3-G3</f>
+        <f t="shared" ref="N3:N16" si="6">$H3-G3</f>
         <v>-8.0500000000000682E-2</v>
       </c>
     </row>
@@ -6914,31 +6947,31 @@
         <v>23.292000000000002</v>
       </c>
       <c r="H4" s="3">
-        <f>AVERAGE(B4:G4)</f>
+        <f t="shared" si="0"/>
         <v>23.195999999999998</v>
       </c>
       <c r="I4" s="3">
-        <f t="shared" si="0"/>
-        <v>-9.6000000000003638E-2</v>
-      </c>
-      <c r="J4" s="3">
         <f t="shared" si="1"/>
         <v>-9.6000000000003638E-2</v>
       </c>
+      <c r="J4" s="3">
+        <f t="shared" si="2"/>
+        <v>-9.6000000000003638E-2</v>
+      </c>
       <c r="K4" s="3">
-        <f t="shared" si="2"/>
-        <v>9.5999999999996533E-2</v>
-      </c>
-      <c r="L4" s="3">
         <f t="shared" si="3"/>
         <v>9.5999999999996533E-2</v>
       </c>
-      <c r="M4" s="3">
+      <c r="L4" s="3">
         <f t="shared" si="4"/>
         <v>9.5999999999996533E-2</v>
       </c>
+      <c r="M4" s="3">
+        <f t="shared" si="5"/>
+        <v>9.5999999999996533E-2</v>
+      </c>
       <c r="N4" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-9.6000000000003638E-2</v>
       </c>
     </row>
@@ -6965,31 +6998,31 @@
         <v>22.428999999999998</v>
       </c>
       <c r="H5" s="3">
-        <f>AVERAGE(B5:G5)</f>
+        <f t="shared" si="0"/>
         <v>22.094333333333335</v>
       </c>
       <c r="I5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.43066666666666364</v>
       </c>
       <c r="J5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4.7666666666664526E-2</v>
       </c>
       <c r="K5" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.33433333333333337</v>
       </c>
       <c r="L5" s="3">
-        <f t="shared" si="3"/>
-        <v>0.23933333333333451</v>
-      </c>
-      <c r="M5" s="3">
         <f t="shared" si="4"/>
         <v>0.23933333333333451</v>
       </c>
+      <c r="M5" s="3">
+        <f t="shared" si="5"/>
+        <v>0.23933333333333451</v>
+      </c>
       <c r="N5" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.33466666666666356</v>
       </c>
     </row>
@@ -7016,31 +7049,31 @@
         <v>21.855</v>
       </c>
       <c r="H6" s="3">
-        <f>AVERAGE(B6:G6)</f>
+        <f t="shared" si="0"/>
         <v>21.457333333333334</v>
       </c>
       <c r="I6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.49366666666666603</v>
       </c>
       <c r="J6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.5666666666664497E-2</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.3663333333333334</v>
       </c>
       <c r="L6" s="3">
-        <f t="shared" si="3"/>
-        <v>0.27033333333333331</v>
-      </c>
-      <c r="M6" s="3">
         <f t="shared" si="4"/>
         <v>0.27033333333333331</v>
       </c>
+      <c r="M6" s="3">
+        <f t="shared" si="5"/>
+        <v>0.27033333333333331</v>
+      </c>
       <c r="N6" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.39766666666666595</v>
       </c>
     </row>
@@ -7067,31 +7100,31 @@
         <v>21.378</v>
       </c>
       <c r="H7" s="3">
-        <f>AVERAGE(B7:G7)</f>
+        <f t="shared" si="0"/>
         <v>20.980333333333331</v>
       </c>
       <c r="I7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.3976666666666695</v>
       </c>
       <c r="J7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.566666666666805E-2</v>
       </c>
       <c r="K7" s="3">
-        <f t="shared" si="2"/>
-        <v>0.27033333333332976</v>
-      </c>
-      <c r="L7" s="3">
         <f t="shared" si="3"/>
         <v>0.27033333333332976</v>
       </c>
-      <c r="M7" s="3">
+      <c r="L7" s="3">
         <f t="shared" si="4"/>
         <v>0.27033333333332976</v>
       </c>
+      <c r="M7" s="3">
+        <f t="shared" si="5"/>
+        <v>0.27033333333332976</v>
+      </c>
       <c r="N7" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.3976666666666695</v>
       </c>
     </row>
@@ -7118,31 +7151,31 @@
         <v>20.901</v>
       </c>
       <c r="H8" s="3">
-        <f>AVERAGE(B8:G8)</f>
+        <f t="shared" si="0"/>
         <v>20.630666666666666</v>
       </c>
       <c r="I8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.36533333333333218</v>
       </c>
       <c r="J8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.566666666666805E-2</v>
       </c>
       <c r="K8" s="3">
-        <f t="shared" si="2"/>
-        <v>0.206666666666667</v>
-      </c>
-      <c r="L8" s="3">
         <f t="shared" si="3"/>
         <v>0.206666666666667</v>
       </c>
-      <c r="M8" s="3">
+      <c r="L8" s="3">
         <f t="shared" si="4"/>
         <v>0.206666666666667</v>
       </c>
+      <c r="M8" s="3">
+        <f t="shared" si="5"/>
+        <v>0.206666666666667</v>
+      </c>
       <c r="N8" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.27033333333333331</v>
       </c>
     </row>
@@ -7169,31 +7202,31 @@
         <v>20.614999999999998</v>
       </c>
       <c r="H9" s="3">
-        <f>AVERAGE(B9:G9)</f>
+        <f t="shared" si="0"/>
         <v>20.344833333333334</v>
       </c>
       <c r="I9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.27016666666666467</v>
       </c>
       <c r="J9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5833333333333144E-2</v>
       </c>
       <c r="K9" s="3">
-        <f t="shared" si="2"/>
-        <v>0.20683333333333209</v>
-      </c>
-      <c r="L9" s="3">
         <f t="shared" si="3"/>
         <v>0.20683333333333209</v>
       </c>
+      <c r="L9" s="3">
+        <f t="shared" si="4"/>
+        <v>0.20683333333333209</v>
+      </c>
       <c r="M9" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.11083333333333201</v>
       </c>
       <c r="N9" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.27016666666666467</v>
       </c>
     </row>
@@ -7220,31 +7253,31 @@
         <v>20.329000000000001</v>
       </c>
       <c r="H10" s="3">
-        <f>AVERAGE(B10:G10)</f>
+        <f t="shared" si="0"/>
         <v>20.106666666666669</v>
       </c>
       <c r="I10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.2223333333333315</v>
       </c>
       <c r="J10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3.1333333333332547E-2</v>
       </c>
       <c r="K10" s="3">
-        <f t="shared" si="2"/>
-        <v>0.15866666666666873</v>
-      </c>
-      <c r="L10" s="3">
         <f t="shared" si="3"/>
         <v>0.15866666666666873</v>
       </c>
-      <c r="M10" s="3">
+      <c r="L10" s="3">
         <f t="shared" si="4"/>
         <v>0.15866666666666873</v>
       </c>
+      <c r="M10" s="3">
+        <f t="shared" si="5"/>
+        <v>0.15866666666666873</v>
+      </c>
       <c r="N10" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.2223333333333315</v>
       </c>
     </row>
@@ -7271,31 +7304,31 @@
         <v>20.042999999999999</v>
       </c>
       <c r="H11" s="3">
-        <f>AVERAGE(B11:G11)</f>
+        <f t="shared" si="0"/>
         <v>19.884666666666664</v>
       </c>
       <c r="I11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.15833333333333499</v>
       </c>
       <c r="J11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-6.3333333333336128E-2</v>
       </c>
       <c r="K11" s="3">
-        <f t="shared" si="2"/>
-        <v>0.12666666666666515</v>
-      </c>
-      <c r="L11" s="3">
         <f t="shared" si="3"/>
         <v>0.12666666666666515</v>
       </c>
-      <c r="M11" s="3">
+      <c r="L11" s="3">
         <f t="shared" si="4"/>
         <v>0.12666666666666515</v>
       </c>
+      <c r="M11" s="3">
+        <f t="shared" si="5"/>
+        <v>0.12666666666666515</v>
+      </c>
       <c r="N11" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.15833333333333499</v>
       </c>
     </row>
@@ -7322,31 +7355,31 @@
         <v>19.853000000000002</v>
       </c>
       <c r="H12" s="3">
-        <f>AVERAGE(B12:G12)</f>
+        <f t="shared" si="0"/>
         <v>19.694166666666671</v>
       </c>
       <c r="I12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.15883333333333027</v>
       </c>
       <c r="J12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-6.3833333333327857E-2</v>
       </c>
       <c r="K12" s="3">
-        <f t="shared" si="2"/>
-        <v>0.12716666666667109</v>
-      </c>
-      <c r="L12" s="3">
         <f t="shared" si="3"/>
         <v>0.12716666666667109</v>
       </c>
-      <c r="M12" s="3">
+      <c r="L12" s="3">
         <f t="shared" si="4"/>
         <v>0.12716666666667109</v>
       </c>
+      <c r="M12" s="3">
+        <f t="shared" si="5"/>
+        <v>0.12716666666667109</v>
+      </c>
       <c r="N12" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.15883333333333027</v>
       </c>
     </row>
@@ -7373,31 +7406,31 @@
         <v>19.567</v>
       </c>
       <c r="H13" s="3">
-        <f>AVERAGE(B13:G13)</f>
+        <f t="shared" si="0"/>
         <v>19.519500000000004</v>
       </c>
       <c r="I13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.14249999999999474</v>
       </c>
       <c r="J13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4.7499999999995879E-2</v>
       </c>
       <c r="K13" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.7500000000002984E-2</v>
       </c>
       <c r="L13" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.1425000000000054</v>
       </c>
       <c r="M13" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.7500000000002984E-2</v>
       </c>
       <c r="N13" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-4.7499999999995879E-2</v>
       </c>
     </row>
@@ -7424,31 +7457,31 @@
         <v>19.472000000000001</v>
       </c>
       <c r="H14" s="3">
-        <f>AVERAGE(B14:G14)</f>
+        <f t="shared" si="0"/>
         <v>19.345333333333333</v>
       </c>
       <c r="I14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.1266666666666687</v>
       </c>
       <c r="J14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3.1666666666666288E-2</v>
       </c>
       <c r="K14" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.3333333333332575E-2</v>
       </c>
       <c r="L14" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.15833333333333144</v>
       </c>
       <c r="M14" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.3333333333332575E-2</v>
       </c>
       <c r="N14" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.1266666666666687</v>
       </c>
     </row>
@@ -7475,31 +7508,31 @@
         <v>19.091999999999999</v>
       </c>
       <c r="H15" s="3">
-        <f>AVERAGE(B15:G15)</f>
+        <f t="shared" si="0"/>
         <v>19.107499999999998</v>
       </c>
       <c r="I15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.17450000000000188</v>
       </c>
       <c r="J15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-7.9500000000003013E-2</v>
       </c>
       <c r="K15" s="3">
-        <f t="shared" si="2"/>
-        <v>0.11149999999999949</v>
-      </c>
-      <c r="L15" s="3">
         <f t="shared" si="3"/>
         <v>0.11149999999999949</v>
       </c>
+      <c r="L15" s="3">
+        <f t="shared" si="4"/>
+        <v>0.11149999999999949</v>
+      </c>
       <c r="M15" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.5499999999999403E-2</v>
       </c>
       <c r="N15" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5499999999999403E-2</v>
       </c>
     </row>
@@ -7526,31 +7559,31 @@
         <v>18.710999999999999</v>
       </c>
       <c r="H16" s="3">
-        <f>AVERAGE(B16:G16)</f>
+        <f t="shared" si="0"/>
         <v>18.679333333333332</v>
       </c>
       <c r="I16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.1266666666666687</v>
       </c>
       <c r="J16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3.1666666666666288E-2</v>
       </c>
       <c r="K16" s="3">
-        <f t="shared" si="2"/>
-        <v>6.3333333333332575E-2</v>
-      </c>
-      <c r="L16" s="3">
         <f t="shared" si="3"/>
         <v>6.3333333333332575E-2</v>
       </c>
-      <c r="M16" s="3">
+      <c r="L16" s="3">
         <f t="shared" si="4"/>
         <v>6.3333333333332575E-2</v>
       </c>
+      <c r="M16" s="3">
+        <f t="shared" si="5"/>
+        <v>6.3333333333332575E-2</v>
+      </c>
       <c r="N16" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-3.1666666666666288E-2</v>
       </c>
     </row>
@@ -7577,15 +7610,15 @@
         <v>18.331</v>
       </c>
       <c r="H17" s="3">
-        <f>AVERAGE(B17:G17)</f>
+        <f t="shared" si="0"/>
         <v>18.267333333333337</v>
       </c>
       <c r="I17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.15866666666666163</v>
       </c>
       <c r="J17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-6.3666666666662763E-2</v>
       </c>
       <c r="K17" s="3">
@@ -7593,11 +7626,11 @@
         <v>0.12733333333333618</v>
       </c>
       <c r="L17" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.12733333333333618</v>
       </c>
       <c r="M17" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.13333333333361E-2</v>
       </c>
       <c r="N17" s="3">
@@ -7628,31 +7661,31 @@
         <v>17.95</v>
       </c>
       <c r="H18" s="3">
-        <f>AVERAGE(B18:G18)</f>
+        <f t="shared" si="0"/>
         <v>17.870833333333337</v>
       </c>
       <c r="I18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.17416666666666458</v>
       </c>
       <c r="J18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-7.9166666666662167E-2</v>
       </c>
       <c r="K18" s="3">
-        <f t="shared" ref="K18:K74" si="6">$H18-D18</f>
+        <f t="shared" ref="K18:K74" si="7">$H18-D18</f>
         <v>0.11083333333333556</v>
       </c>
       <c r="L18" s="3">
-        <f t="shared" ref="L18:L74" si="7">$H18-E18</f>
+        <f t="shared" ref="L18:L74" si="8">$H18-E18</f>
         <v>0.11083333333333556</v>
       </c>
       <c r="M18" s="3">
-        <f t="shared" ref="M18:M74" si="8">$H18-F18</f>
+        <f t="shared" ref="M18:M74" si="9">$H18-F18</f>
         <v>0.11083333333333556</v>
       </c>
       <c r="N18" s="3">
-        <f t="shared" ref="N18:N74" si="9">$H18-G18</f>
+        <f t="shared" ref="N18:N74" si="10">$H18-G18</f>
         <v>-7.9166666666662167E-2</v>
       </c>
     </row>
@@ -7679,31 +7712,31 @@
         <v>17.57</v>
       </c>
       <c r="H19" s="3">
-        <f>AVERAGE(B19:G19)</f>
+        <f t="shared" si="0"/>
         <v>17.490333333333336</v>
       </c>
       <c r="I19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.17466666666666342</v>
       </c>
       <c r="J19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-7.9666666666664554E-2</v>
       </c>
       <c r="K19" s="3">
-        <f t="shared" si="6"/>
-        <v>0.11133333333333439</v>
-      </c>
-      <c r="L19" s="3">
         <f t="shared" si="7"/>
         <v>0.11133333333333439</v>
       </c>
-      <c r="M19" s="3">
+      <c r="L19" s="3">
         <f t="shared" si="8"/>
         <v>0.11133333333333439</v>
       </c>
+      <c r="M19" s="3">
+        <f t="shared" si="9"/>
+        <v>0.11133333333333439</v>
+      </c>
       <c r="N19" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-7.9666666666664554E-2</v>
       </c>
     </row>
@@ -7730,31 +7763,31 @@
         <v>17.189</v>
       </c>
       <c r="H20" s="3">
-        <f>AVERAGE(B20:G20)</f>
+        <f t="shared" si="0"/>
         <v>17.109833333333331</v>
       </c>
       <c r="I20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.17416666666666814</v>
       </c>
       <c r="J20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-7.9166666666669272E-2</v>
       </c>
       <c r="K20" s="3">
-        <f t="shared" si="6"/>
-        <v>0.11083333333333201</v>
-      </c>
-      <c r="L20" s="3">
         <f t="shared" si="7"/>
         <v>0.11083333333333201</v>
       </c>
-      <c r="M20" s="3">
+      <c r="L20" s="3">
         <f t="shared" si="8"/>
         <v>0.11083333333333201</v>
       </c>
+      <c r="M20" s="3">
+        <f t="shared" si="9"/>
+        <v>0.11083333333333201</v>
+      </c>
       <c r="N20" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-7.9166666666669272E-2</v>
       </c>
     </row>
@@ -7781,31 +7814,31 @@
         <v>16.808</v>
       </c>
       <c r="H21" s="3">
-        <f>AVERAGE(B21:G21)</f>
+        <f t="shared" si="0"/>
         <v>16.760499999999997</v>
       </c>
       <c r="I21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.14250000000000185</v>
       </c>
       <c r="J21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4.7500000000002984E-2</v>
       </c>
       <c r="K21" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.7499999999995879E-2</v>
       </c>
       <c r="L21" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.14249999999999829</v>
       </c>
       <c r="M21" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.7499999999995879E-2</v>
       </c>
       <c r="N21" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-4.7500000000002984E-2</v>
       </c>
     </row>
@@ -7832,31 +7865,31 @@
         <v>16.523</v>
       </c>
       <c r="H22" s="3">
-        <f>AVERAGE(B22:G22)</f>
+        <f t="shared" si="0"/>
         <v>16.427333333333333</v>
       </c>
       <c r="I22" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.19066666666666521</v>
       </c>
       <c r="J22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.3333333333374071E-4</v>
       </c>
       <c r="K22" s="3">
-        <f t="shared" si="6"/>
-        <v>9.5333333333332604E-2</v>
-      </c>
-      <c r="L22" s="3">
         <f t="shared" si="7"/>
         <v>9.5333333333332604E-2</v>
       </c>
-      <c r="M22" s="3">
+      <c r="L22" s="3">
         <f t="shared" si="8"/>
         <v>9.5333333333332604E-2</v>
       </c>
+      <c r="M22" s="3">
+        <f t="shared" si="9"/>
+        <v>9.5333333333332604E-2</v>
+      </c>
       <c r="N22" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-9.5666666666666345E-2</v>
       </c>
     </row>
@@ -7883,31 +7916,31 @@
         <v>16.140999999999998</v>
       </c>
       <c r="H23" s="3">
-        <f>AVERAGE(B23:G23)</f>
+        <f t="shared" si="0"/>
         <v>16.061999999999998</v>
       </c>
       <c r="I23" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.17500000000000071</v>
       </c>
       <c r="J23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-7.9000000000000625E-2</v>
       </c>
       <c r="K23" s="3">
-        <f t="shared" si="6"/>
-        <v>0.1109999999999971</v>
-      </c>
-      <c r="L23" s="3">
         <f t="shared" si="7"/>
         <v>0.1109999999999971</v>
       </c>
-      <c r="M23" s="3">
+      <c r="L23" s="3">
         <f t="shared" si="8"/>
         <v>0.1109999999999971</v>
       </c>
+      <c r="M23" s="3">
+        <f t="shared" si="9"/>
+        <v>0.1109999999999971</v>
+      </c>
       <c r="N23" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-7.9000000000000625E-2</v>
       </c>
     </row>
@@ -7934,31 +7967,31 @@
         <v>15.855</v>
       </c>
       <c r="H24" s="3">
-        <f>AVERAGE(B24:G24)</f>
+        <f t="shared" si="0"/>
         <v>15.775500000000001</v>
       </c>
       <c r="I24" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.17549999999999955</v>
       </c>
       <c r="J24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-7.949999999999946E-2</v>
       </c>
       <c r="K24" s="3">
-        <f t="shared" si="6"/>
-        <v>0.11150000000000126</v>
-      </c>
-      <c r="L24" s="3">
         <f t="shared" si="7"/>
         <v>0.11150000000000126</v>
       </c>
-      <c r="M24" s="3">
+      <c r="L24" s="3">
         <f t="shared" si="8"/>
         <v>0.11150000000000126</v>
       </c>
+      <c r="M24" s="3">
+        <f t="shared" si="9"/>
+        <v>0.11150000000000126</v>
+      </c>
       <c r="N24" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-7.949999999999946E-2</v>
       </c>
     </row>
@@ -7985,31 +8018,31 @@
         <v>15.569000000000001</v>
       </c>
       <c r="H25" s="3">
-        <f>AVERAGE(B25:G25)</f>
+        <f t="shared" si="0"/>
         <v>15.489333333333335</v>
       </c>
       <c r="I25" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.17466666666666519</v>
       </c>
       <c r="J25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-7.966666666666633E-2</v>
       </c>
       <c r="K25" s="3">
-        <f t="shared" si="6"/>
-        <v>0.11133333333333439</v>
-      </c>
-      <c r="L25" s="3">
         <f t="shared" si="7"/>
         <v>0.11133333333333439</v>
       </c>
-      <c r="M25" s="3">
+      <c r="L25" s="3">
         <f t="shared" si="8"/>
         <v>0.11133333333333439</v>
       </c>
+      <c r="M25" s="3">
+        <f t="shared" si="9"/>
+        <v>0.11133333333333439</v>
+      </c>
       <c r="N25" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-7.966666666666633E-2</v>
       </c>
     </row>
@@ -8036,31 +8069,31 @@
         <v>15.282</v>
       </c>
       <c r="H26" s="3">
-        <f>AVERAGE(B26:G26)</f>
+        <f t="shared" si="0"/>
         <v>15.218499999999999</v>
       </c>
       <c r="I26" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.15950000000000131</v>
       </c>
       <c r="J26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-6.3500000000001222E-2</v>
       </c>
       <c r="K26" s="3">
-        <f t="shared" si="6"/>
-        <v>0.1274999999999995</v>
-      </c>
-      <c r="L26" s="3">
         <f t="shared" si="7"/>
         <v>0.1274999999999995</v>
       </c>
+      <c r="L26" s="3">
+        <f t="shared" si="8"/>
+        <v>0.1274999999999995</v>
+      </c>
       <c r="M26" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.1499999999999417E-2</v>
       </c>
       <c r="N26" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-6.3500000000001222E-2</v>
       </c>
     </row>
@@ -8087,31 +8120,31 @@
         <v>15.090999999999999</v>
       </c>
       <c r="H27" s="3">
-        <f>AVERAGE(B27:G27)</f>
+        <f t="shared" si="0"/>
         <v>14.995666666666665</v>
       </c>
       <c r="I27" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.19133333333333447</v>
       </c>
       <c r="J27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3.3333333333551707E-4</v>
       </c>
       <c r="K27" s="3">
-        <f t="shared" si="6"/>
-        <v>9.5666666666664568E-2</v>
-      </c>
-      <c r="L27" s="3">
         <f t="shared" si="7"/>
         <v>9.5666666666664568E-2</v>
       </c>
-      <c r="M27" s="3">
+      <c r="L27" s="3">
         <f t="shared" si="8"/>
         <v>9.5666666666664568E-2</v>
       </c>
+      <c r="M27" s="3">
+        <f t="shared" si="9"/>
+        <v>9.5666666666664568E-2</v>
+      </c>
       <c r="N27" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-9.533333333333438E-2</v>
       </c>
     </row>
@@ -8138,31 +8171,31 @@
         <v>14.804</v>
       </c>
       <c r="H28" s="3">
-        <f>AVERAGE(B28:G28)</f>
+        <f t="shared" si="0"/>
         <v>14.788333333333334</v>
       </c>
       <c r="I28" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.11166666666666636</v>
       </c>
       <c r="J28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.5666666666666273E-2</v>
       </c>
       <c r="K28" s="3">
-        <f t="shared" si="6"/>
-        <v>7.9333333333334366E-2</v>
-      </c>
-      <c r="L28" s="3">
         <f t="shared" si="7"/>
         <v>7.9333333333334366E-2</v>
       </c>
+      <c r="L28" s="3">
+        <f t="shared" si="8"/>
+        <v>7.9333333333334366E-2</v>
+      </c>
       <c r="M28" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1.5666666666666273E-2</v>
       </c>
       <c r="N28" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.5666666666666273E-2</v>
       </c>
     </row>
@@ -8189,31 +8222,31 @@
         <v>14.709</v>
       </c>
       <c r="H29" s="3">
-        <f>AVERAGE(B29:G29)</f>
+        <f t="shared" si="0"/>
         <v>14.645000000000001</v>
       </c>
       <c r="I29" s="3">
-        <f t="shared" si="0"/>
-        <v>-6.399999999999828E-2</v>
-      </c>
-      <c r="J29" s="3">
         <f t="shared" si="1"/>
         <v>-6.399999999999828E-2</v>
       </c>
+      <c r="J29" s="3">
+        <f t="shared" si="2"/>
+        <v>-6.399999999999828E-2</v>
+      </c>
       <c r="K29" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.2000000000001805E-2</v>
       </c>
       <c r="L29" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.12800000000000189</v>
       </c>
       <c r="M29" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.2000000000001805E-2</v>
       </c>
       <c r="N29" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-6.399999999999828E-2</v>
       </c>
     </row>
@@ -8240,31 +8273,31 @@
         <v>14.516999999999999</v>
       </c>
       <c r="H30" s="3">
-        <f>AVERAGE(B30:G30)</f>
+        <f t="shared" si="0"/>
         <v>14.468999999999999</v>
       </c>
       <c r="I30" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.14400000000000013</v>
       </c>
       <c r="J30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4.8000000000000043E-2</v>
       </c>
       <c r="K30" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="L30" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.14400000000000013</v>
       </c>
       <c r="M30" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="N30" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-4.8000000000000043E-2</v>
       </c>
     </row>
@@ -8291,31 +8324,31 @@
         <v>14.324999999999999</v>
       </c>
       <c r="H31" s="3">
-        <f>AVERAGE(B31:G31)</f>
+        <f t="shared" si="0"/>
         <v>14.277500000000002</v>
       </c>
       <c r="I31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.14349999999999774</v>
       </c>
       <c r="J31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4.7499999999997655E-2</v>
       </c>
       <c r="K31" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.7500000000001208E-2</v>
       </c>
       <c r="L31" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.14350000000000129</v>
       </c>
       <c r="M31" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.7500000000001208E-2</v>
       </c>
       <c r="N31" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-4.7499999999997655E-2</v>
       </c>
     </row>
@@ -8342,31 +8375,31 @@
         <v>14.134</v>
       </c>
       <c r="H32" s="3">
-        <f>AVERAGE(B32:G32)</f>
+        <f t="shared" si="0"/>
         <v>14.118</v>
       </c>
       <c r="I32" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.1120000000000001</v>
       </c>
       <c r="J32" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.6000000000000014E-2</v>
       </c>
       <c r="K32" s="3">
-        <f t="shared" si="6"/>
-        <v>8.0000000000000071E-2</v>
-      </c>
-      <c r="L32" s="3">
         <f t="shared" si="7"/>
         <v>8.0000000000000071E-2</v>
       </c>
+      <c r="L32" s="3">
+        <f t="shared" si="8"/>
+        <v>8.0000000000000071E-2</v>
+      </c>
       <c r="M32" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1.6000000000000014E-2</v>
       </c>
       <c r="N32" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.6000000000000014E-2</v>
       </c>
     </row>
@@ -8393,31 +8426,31 @@
         <v>14.038</v>
       </c>
       <c r="H33" s="3">
-        <f>AVERAGE(B33:G33)</f>
+        <f t="shared" si="0"/>
         <v>13.974000000000002</v>
       </c>
       <c r="I33" s="3">
-        <f t="shared" si="0"/>
-        <v>-6.399999999999828E-2</v>
-      </c>
-      <c r="J33" s="3">
         <f t="shared" si="1"/>
         <v>-6.399999999999828E-2</v>
       </c>
+      <c r="J33" s="3">
+        <f t="shared" si="2"/>
+        <v>-6.399999999999828E-2</v>
+      </c>
       <c r="K33" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.2000000000001805E-2</v>
       </c>
       <c r="L33" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.12800000000000189</v>
       </c>
       <c r="M33" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.2000000000001805E-2</v>
       </c>
       <c r="N33" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-6.399999999999828E-2</v>
       </c>
     </row>
@@ -8444,31 +8477,31 @@
         <v>13.846</v>
       </c>
       <c r="H34" s="3">
-        <f>AVERAGE(B34:G34)</f>
+        <f t="shared" ref="H34:H65" si="11">AVERAGE(B34:G34)</f>
         <v>13.862000000000002</v>
       </c>
       <c r="I34" s="3">
-        <f t="shared" si="0"/>
-        <v>-7.9999999999998295E-2</v>
-      </c>
-      <c r="J34" s="3">
         <f t="shared" si="1"/>
         <v>-7.9999999999998295E-2</v>
       </c>
+      <c r="J34" s="3">
+        <f t="shared" si="2"/>
+        <v>-7.9999999999998295E-2</v>
+      </c>
       <c r="K34" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6000000000001791E-2</v>
       </c>
       <c r="L34" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.11200000000000188</v>
       </c>
       <c r="M34" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.6000000000001791E-2</v>
       </c>
       <c r="N34" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.6000000000001791E-2</v>
       </c>
     </row>
@@ -8495,31 +8528,31 @@
         <v>13.75</v>
       </c>
       <c r="H35" s="3">
-        <f>AVERAGE(B35:G35)</f>
+        <f t="shared" si="11"/>
         <v>13.702</v>
       </c>
       <c r="I35" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.14400000000000013</v>
       </c>
       <c r="J35" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4.8000000000000043E-2</v>
       </c>
       <c r="K35" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="L35" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.14400000000000013</v>
       </c>
       <c r="M35" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="N35" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-4.8000000000000043E-2</v>
       </c>
     </row>
@@ -8546,31 +8579,31 @@
         <v>13.654</v>
       </c>
       <c r="H36" s="3">
-        <f>AVERAGE(B36:G36)</f>
+        <f t="shared" si="11"/>
         <v>13.589833333333331</v>
       </c>
       <c r="I36" s="3">
-        <f t="shared" si="0"/>
-        <v>-6.4166666666668704E-2</v>
-      </c>
-      <c r="J36" s="3">
         <f t="shared" si="1"/>
         <v>-6.4166666666668704E-2</v>
       </c>
+      <c r="J36" s="3">
+        <f t="shared" si="2"/>
+        <v>-6.4166666666668704E-2</v>
+      </c>
       <c r="K36" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.1833333333331382E-2</v>
       </c>
       <c r="L36" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.12883333333333091</v>
       </c>
       <c r="M36" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.1833333333331382E-2</v>
       </c>
       <c r="N36" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-6.4166666666668704E-2</v>
       </c>
     </row>
@@ -8597,31 +8630,31 @@
         <v>13.461</v>
       </c>
       <c r="H37" s="3">
-        <f>AVERAGE(B37:G37)</f>
+        <f t="shared" si="11"/>
         <v>13.477333333333334</v>
       </c>
       <c r="I37" s="3">
-        <f t="shared" si="0"/>
-        <v>-8.0666666666665776E-2</v>
-      </c>
-      <c r="J37" s="3">
         <f t="shared" si="1"/>
         <v>-8.0666666666665776E-2</v>
       </c>
+      <c r="J37" s="3">
+        <f t="shared" si="2"/>
+        <v>-8.0666666666665776E-2</v>
+      </c>
       <c r="K37" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6333333333333755E-2</v>
       </c>
       <c r="L37" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.11233333333333384</v>
       </c>
       <c r="M37" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.6333333333333755E-2</v>
       </c>
       <c r="N37" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.6333333333333755E-2</v>
       </c>
     </row>
@@ -8648,31 +8681,31 @@
         <v>13.365</v>
       </c>
       <c r="H38" s="3">
-        <f>AVERAGE(B38:G38)</f>
+        <f t="shared" si="11"/>
         <v>13.365</v>
       </c>
       <c r="I38" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-9.6000000000000085E-2</v>
       </c>
       <c r="J38" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K38" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L38" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9.6000000000000085E-2</v>
       </c>
       <c r="M38" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N38" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -8699,31 +8732,31 @@
         <v>13.269</v>
       </c>
       <c r="H39" s="3">
-        <f>AVERAGE(B39:G39)</f>
+        <f t="shared" si="11"/>
         <v>13.285000000000002</v>
       </c>
       <c r="I39" s="3">
-        <f t="shared" si="0"/>
-        <v>-7.9999999999998295E-2</v>
-      </c>
-      <c r="J39" s="3">
         <f t="shared" si="1"/>
         <v>-7.9999999999998295E-2</v>
       </c>
+      <c r="J39" s="3">
+        <f t="shared" si="2"/>
+        <v>-7.9999999999998295E-2</v>
+      </c>
       <c r="K39" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6000000000001791E-2</v>
       </c>
       <c r="L39" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.11200000000000188</v>
       </c>
       <c r="M39" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.6000000000001791E-2</v>
       </c>
       <c r="N39" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.6000000000001791E-2</v>
       </c>
     </row>
@@ -8750,31 +8783,31 @@
         <v>13.269</v>
       </c>
       <c r="H40" s="3">
-        <f>AVERAGE(B40:G40)</f>
+        <f t="shared" si="11"/>
         <v>13.204833333333333</v>
       </c>
       <c r="I40" s="3">
-        <f t="shared" si="0"/>
-        <v>-6.4166666666666927E-2</v>
-      </c>
-      <c r="J40" s="3">
         <f t="shared" si="1"/>
         <v>-6.4166666666666927E-2</v>
       </c>
+      <c r="J40" s="3">
+        <f t="shared" si="2"/>
+        <v>-6.4166666666666927E-2</v>
+      </c>
       <c r="K40" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.1833333333333158E-2</v>
       </c>
       <c r="L40" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.12883333333333269</v>
       </c>
       <c r="M40" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.1833333333333158E-2</v>
       </c>
       <c r="N40" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-6.4166666666666927E-2</v>
       </c>
     </row>
@@ -8801,31 +8834,31 @@
         <v>13.173</v>
       </c>
       <c r="H41" s="3">
-        <f>AVERAGE(B41:G41)</f>
+        <f t="shared" si="11"/>
         <v>13.108500000000001</v>
       </c>
       <c r="I41" s="3">
-        <f t="shared" si="0"/>
-        <v>-6.4499999999998892E-2</v>
-      </c>
-      <c r="J41" s="3">
         <f t="shared" si="1"/>
         <v>-6.4499999999998892E-2</v>
       </c>
+      <c r="J41" s="3">
+        <f t="shared" si="2"/>
+        <v>-6.4499999999998892E-2</v>
+      </c>
       <c r="K41" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.2500000000000639E-2</v>
       </c>
       <c r="L41" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.12850000000000072</v>
       </c>
       <c r="M41" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.2500000000000639E-2</v>
       </c>
       <c r="N41" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-6.4499999999998892E-2</v>
       </c>
     </row>
@@ -8852,31 +8885,31 @@
         <v>13.076000000000001</v>
       </c>
       <c r="H42" s="3">
-        <f>AVERAGE(B42:G42)</f>
+        <f t="shared" si="11"/>
         <v>13.027833333333334</v>
       </c>
       <c r="I42" s="3">
-        <f t="shared" si="0"/>
-        <v>-4.8166666666666913E-2</v>
-      </c>
-      <c r="J42" s="3">
         <f t="shared" si="1"/>
         <v>-4.8166666666666913E-2</v>
       </c>
+      <c r="J42" s="3">
+        <f t="shared" si="2"/>
+        <v>-4.8166666666666913E-2</v>
+      </c>
       <c r="K42" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.7833333333333172E-2</v>
       </c>
       <c r="L42" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.14483333333333448</v>
       </c>
       <c r="M42" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.8166666666666913E-2</v>
       </c>
       <c r="N42" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-4.8166666666666913E-2</v>
       </c>
     </row>
@@ -8903,31 +8936,31 @@
         <v>13.076000000000001</v>
       </c>
       <c r="H43" s="3">
-        <f>AVERAGE(B43:G43)</f>
+        <f t="shared" si="11"/>
         <v>13.027833333333334</v>
       </c>
       <c r="I43" s="3">
-        <f t="shared" si="0"/>
-        <v>-4.8166666666666913E-2</v>
-      </c>
-      <c r="J43" s="3">
         <f t="shared" si="1"/>
         <v>-4.8166666666666913E-2</v>
       </c>
+      <c r="J43" s="3">
+        <f t="shared" si="2"/>
+        <v>-4.8166666666666913E-2</v>
+      </c>
       <c r="K43" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.7833333333333172E-2</v>
       </c>
       <c r="L43" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.14483333333333448</v>
       </c>
       <c r="M43" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.8166666666666913E-2</v>
       </c>
       <c r="N43" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-4.8166666666666913E-2</v>
       </c>
     </row>
@@ -8954,31 +8987,31 @@
         <v>13.173</v>
       </c>
       <c r="H44" s="3">
-        <f>AVERAGE(B44:G44)</f>
+        <f t="shared" si="11"/>
         <v>13.092333333333334</v>
       </c>
       <c r="I44" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-8.0666666666665776E-2</v>
       </c>
       <c r="J44" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6333333333333755E-2</v>
       </c>
       <c r="K44" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6333333333333755E-2</v>
       </c>
       <c r="L44" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.11233333333333384</v>
       </c>
       <c r="M44" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.6333333333333755E-2</v>
       </c>
       <c r="N44" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-8.0666666666665776E-2</v>
       </c>
     </row>
@@ -9005,31 +9038,31 @@
         <v>13.269</v>
       </c>
       <c r="H45" s="3">
-        <f>AVERAGE(B45:G45)</f>
+        <f t="shared" si="11"/>
         <v>13.188833333333335</v>
       </c>
       <c r="I45" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-8.0166666666665165E-2</v>
       </c>
       <c r="J45" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.583333333333492E-2</v>
       </c>
       <c r="K45" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.583333333333492E-2</v>
       </c>
       <c r="L45" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.20883333333333454</v>
       </c>
       <c r="M45" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-8.0166666666665165E-2</v>
       </c>
       <c r="N45" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-8.0166666666665165E-2</v>
       </c>
     </row>
@@ -9056,31 +9089,31 @@
         <v>13.365</v>
       </c>
       <c r="H46" s="3">
-        <f>AVERAGE(B46:G46)</f>
+        <f t="shared" si="11"/>
         <v>13.317</v>
       </c>
       <c r="I46" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-4.8000000000000043E-2</v>
       </c>
       <c r="J46" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="K46" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-4.8000000000000043E-2</v>
       </c>
       <c r="L46" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.14400000000000013</v>
       </c>
       <c r="M46" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.8000000000000043E-2</v>
       </c>
       <c r="N46" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-4.8000000000000043E-2</v>
       </c>
     </row>
@@ -9107,31 +9140,31 @@
         <v>13.558</v>
       </c>
       <c r="H47" s="3">
-        <f>AVERAGE(B47:G47)</f>
+        <f t="shared" si="11"/>
         <v>13.477499999999997</v>
       </c>
       <c r="I47" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-8.0500000000002458E-2</v>
       </c>
       <c r="J47" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6499999999997073E-2</v>
       </c>
       <c r="K47" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6499999999997073E-2</v>
       </c>
       <c r="L47" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.20849999999999724</v>
       </c>
       <c r="M47" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-8.0500000000002458E-2</v>
       </c>
       <c r="N47" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-8.0500000000002458E-2</v>
       </c>
     </row>
@@ -9158,31 +9191,31 @@
         <v>13.75</v>
       </c>
       <c r="H48" s="3">
-        <f>AVERAGE(B48:G48)</f>
+        <f t="shared" si="11"/>
         <v>13.653833333333333</v>
       </c>
       <c r="I48" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-9.6166666666666956E-2</v>
       </c>
       <c r="J48" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.6666666666687036E-4</v>
       </c>
       <c r="K48" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-1.6666666666687036E-4</v>
       </c>
       <c r="L48" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.19283333333333275</v>
       </c>
       <c r="M48" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1.6666666666687036E-4</v>
       </c>
       <c r="N48" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-9.6166666666666956E-2</v>
       </c>
     </row>
@@ -9209,31 +9242,31 @@
         <v>15.090999999999999</v>
       </c>
       <c r="H49" s="3">
-        <f>AVERAGE(B49:G49)</f>
+        <f t="shared" si="11"/>
         <v>14.756500000000001</v>
       </c>
       <c r="I49" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.14349999999999952</v>
       </c>
       <c r="J49" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.23950000000000138</v>
       </c>
       <c r="K49" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.7500000000001208E-2</v>
       </c>
       <c r="L49" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.14350000000000129</v>
       </c>
       <c r="M49" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.7500000000001208E-2</v>
       </c>
       <c r="N49" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.33449999999999847</v>
       </c>
     </row>
@@ -9260,31 +9293,31 @@
         <v>15.569000000000001</v>
       </c>
       <c r="H50" s="3">
-        <f>AVERAGE(B50:G50)</f>
+        <f t="shared" si="11"/>
         <v>15.282333333333334</v>
       </c>
       <c r="I50" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.19133333333333447</v>
       </c>
       <c r="J50" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.3333333333374071E-4</v>
       </c>
       <c r="K50" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-9.5666666666666345E-2</v>
       </c>
       <c r="L50" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.28633333333333333</v>
       </c>
       <c r="M50" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-9.5666666666666345E-2</v>
       </c>
       <c r="N50" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.28666666666666707</v>
       </c>
     </row>
@@ -9311,31 +9344,31 @@
         <v>15.282</v>
       </c>
       <c r="H51" s="3">
-        <f>AVERAGE(B51:G51)</f>
+        <f t="shared" si="11"/>
         <v>15.170833333333333</v>
       </c>
       <c r="I51" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.17483333333333206</v>
       </c>
       <c r="J51" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.11116666666666752</v>
       </c>
       <c r="K51" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.30216666666666825</v>
       </c>
       <c r="L51" s="3">
-        <f t="shared" si="7"/>
-        <v>0.17483333333333206</v>
-      </c>
-      <c r="M51" s="3">
         <f t="shared" si="8"/>
         <v>0.17483333333333206</v>
       </c>
+      <c r="M51" s="3">
+        <f t="shared" si="9"/>
+        <v>0.17483333333333206</v>
+      </c>
       <c r="N51" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.11116666666666752</v>
       </c>
     </row>
@@ -9362,31 +9395,31 @@
         <v>14.134</v>
       </c>
       <c r="H52" s="3">
-        <f>AVERAGE(B52:G52)</f>
+        <f t="shared" si="11"/>
         <v>14.2295</v>
       </c>
       <c r="I52" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-9.5499999999999474E-2</v>
       </c>
       <c r="J52" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.5499999999999474E-2</v>
       </c>
       <c r="K52" s="3">
-        <f t="shared" si="6"/>
-        <v>-0.19149999999999956</v>
-      </c>
-      <c r="L52" s="3">
         <f t="shared" si="7"/>
         <v>-0.19149999999999956</v>
       </c>
+      <c r="L52" s="3">
+        <f t="shared" si="8"/>
+        <v>-0.19149999999999956</v>
+      </c>
       <c r="M52" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.28749999999999964</v>
       </c>
       <c r="N52" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>9.5499999999999474E-2</v>
       </c>
     </row>
@@ -9413,31 +9446,31 @@
         <v>13.461</v>
       </c>
       <c r="H53" s="3">
-        <f>AVERAGE(B53:G53)</f>
+        <f t="shared" si="11"/>
         <v>13.461166666666665</v>
       </c>
       <c r="I53" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.66666666665094E-4</v>
       </c>
       <c r="J53" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-9.6833333333334437E-2</v>
       </c>
       <c r="K53" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.28883333333333461</v>
       </c>
       <c r="L53" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.66666666665094E-4</v>
       </c>
       <c r="M53" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.38516666666666488</v>
       </c>
       <c r="N53" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.66666666665094E-4</v>
       </c>
     </row>
@@ -9464,31 +9497,31 @@
         <v>12.787000000000001</v>
       </c>
       <c r="H54" s="3">
-        <f>AVERAGE(B54:G54)</f>
+        <f t="shared" si="11"/>
         <v>12.722333333333333</v>
       </c>
       <c r="I54" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.2333333333333769E-2</v>
       </c>
       <c r="J54" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.16066666666666585</v>
       </c>
       <c r="K54" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.25766666666666715</v>
       </c>
       <c r="L54" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.2333333333333769E-2</v>
       </c>
       <c r="M54" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.418333333333333</v>
       </c>
       <c r="N54" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-6.4666666666667538E-2</v>
       </c>
     </row>
@@ -9515,31 +9548,31 @@
         <v>13.076000000000001</v>
       </c>
       <c r="H55" s="3">
-        <f>AVERAGE(B55:G55)</f>
+        <f t="shared" si="11"/>
         <v>12.770833333333334</v>
       </c>
       <c r="I55" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.17683333333333451</v>
       </c>
       <c r="J55" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.2091666666666665</v>
       </c>
       <c r="K55" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.40216666666666612</v>
       </c>
       <c r="L55" s="3">
-        <f t="shared" si="7"/>
-        <v>0.36983333333333412</v>
-      </c>
-      <c r="M55" s="3">
         <f t="shared" si="8"/>
         <v>0.36983333333333412</v>
       </c>
+      <c r="M55" s="3">
+        <f t="shared" si="9"/>
+        <v>0.36983333333333412</v>
+      </c>
       <c r="N55" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.30516666666666659</v>
       </c>
     </row>
@@ -9566,31 +9599,31 @@
         <v>13.269</v>
       </c>
       <c r="H56" s="3">
-        <f>AVERAGE(B56:G56)</f>
+        <f t="shared" si="11"/>
         <v>12.979833333333334</v>
       </c>
       <c r="I56" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.19283333333333275</v>
       </c>
       <c r="J56" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.19316666666666649</v>
       </c>
       <c r="K56" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.28916666666666657</v>
       </c>
       <c r="L56" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.38583333333333414</v>
       </c>
       <c r="M56" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.19283333333333275</v>
       </c>
       <c r="N56" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.28916666666666657</v>
       </c>
     </row>
@@ -9617,31 +9650,31 @@
         <v>13.461</v>
       </c>
       <c r="H57" s="3">
-        <f>AVERAGE(B57:G57)</f>
+        <f t="shared" si="11"/>
         <v>13.268666666666666</v>
       </c>
       <c r="I57" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.19266666666666588</v>
       </c>
       <c r="J57" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.28933333333333344</v>
       </c>
       <c r="K57" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.19233333333333391</v>
       </c>
       <c r="L57" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.38566666666666727</v>
       </c>
       <c r="M57" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>9.5666666666666345E-2</v>
       </c>
       <c r="N57" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.19233333333333391</v>
       </c>
     </row>
@@ -9668,31 +9701,31 @@
         <v>13.461</v>
       </c>
       <c r="H58" s="3">
-        <f>AVERAGE(B58:G58)</f>
+        <f t="shared" si="11"/>
         <v>13.381166666666665</v>
       </c>
       <c r="I58" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.11216666666666519</v>
       </c>
       <c r="J58" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.17683333333333451</v>
       </c>
       <c r="K58" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.17683333333333451</v>
       </c>
       <c r="L58" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.30516666666666481</v>
       </c>
       <c r="M58" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.6166666666665108E-2</v>
       </c>
       <c r="N58" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-7.9833333333334977E-2</v>
       </c>
     </row>
@@ -9719,31 +9752,31 @@
         <v>13.365</v>
       </c>
       <c r="H59" s="3">
-        <f>AVERAGE(B59:G59)</f>
+        <f t="shared" si="11"/>
         <v>13.284999999999998</v>
       </c>
       <c r="I59" s="3">
-        <f t="shared" si="0"/>
-        <v>1.5999999999998238E-2</v>
-      </c>
-      <c r="J59" s="3">
         <f t="shared" si="1"/>
         <v>1.5999999999998238E-2</v>
       </c>
+      <c r="J59" s="3">
+        <f t="shared" si="2"/>
+        <v>1.5999999999998238E-2</v>
+      </c>
       <c r="K59" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.5999999999998238E-2</v>
       </c>
       <c r="L59" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.11199999999999832</v>
       </c>
       <c r="M59" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-8.0000000000001847E-2</v>
       </c>
       <c r="N59" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-8.0000000000001847E-2</v>
       </c>
     </row>
@@ -9770,31 +9803,31 @@
         <v>13.558</v>
       </c>
       <c r="H60" s="3">
-        <f>AVERAGE(B60:G60)</f>
+        <f t="shared" si="11"/>
         <v>13.348999999999998</v>
       </c>
       <c r="I60" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.9999999999998295E-2</v>
       </c>
       <c r="J60" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.6000000000001791E-2</v>
       </c>
       <c r="K60" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-1.6000000000001791E-2</v>
       </c>
       <c r="L60" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.27299999999999791</v>
       </c>
       <c r="M60" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.11200000000000188</v>
       </c>
       <c r="N60" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.20900000000000141</v>
       </c>
     </row>
@@ -9821,31 +9854,31 @@
         <v>13.654</v>
       </c>
       <c r="H61" s="3">
-        <f>AVERAGE(B61:G61)</f>
+        <f t="shared" si="11"/>
         <v>13.461500000000001</v>
       </c>
       <c r="I61" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.6500000000000696E-2</v>
       </c>
       <c r="J61" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.0000000000061107E-4</v>
       </c>
       <c r="K61" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-9.649999999999892E-2</v>
       </c>
       <c r="L61" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.28850000000000087</v>
       </c>
       <c r="M61" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-9.649999999999892E-2</v>
       </c>
       <c r="N61" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.19249999999999901</v>
       </c>
     </row>
@@ -9872,31 +9905,31 @@
         <v>13.846</v>
       </c>
       <c r="H62" s="3">
-        <f>AVERAGE(B62:G62)</f>
+        <f t="shared" si="11"/>
         <v>13.589833333333333</v>
       </c>
       <c r="I62" s="3">
-        <f t="shared" si="0"/>
-        <v>3.1833333333333158E-2</v>
-      </c>
-      <c r="J62" s="3">
         <f t="shared" si="1"/>
         <v>3.1833333333333158E-2</v>
       </c>
+      <c r="J62" s="3">
+        <f t="shared" si="2"/>
+        <v>3.1833333333333158E-2</v>
+      </c>
       <c r="K62" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-6.4166666666666927E-2</v>
       </c>
       <c r="L62" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.32083333333333286</v>
       </c>
       <c r="M62" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-6.4166666666666927E-2</v>
       </c>
       <c r="N62" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.2561666666666671</v>
       </c>
     </row>
@@ -9923,31 +9956,31 @@
         <v>14.038</v>
       </c>
       <c r="H63" s="3">
-        <f>AVERAGE(B63:G63)</f>
+        <f t="shared" si="11"/>
         <v>13.733833333333335</v>
       </c>
       <c r="I63" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.9833333333334977E-2</v>
       </c>
       <c r="J63" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.6166666666665108E-2</v>
       </c>
       <c r="K63" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.11216666666666519</v>
       </c>
       <c r="L63" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.36883333333333468</v>
       </c>
       <c r="M63" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1.6166666666665108E-2</v>
       </c>
       <c r="N63" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.30416666666666536</v>
       </c>
     </row>
@@ -9974,31 +10007,31 @@
         <v>14.324999999999999</v>
       </c>
       <c r="H64" s="3">
-        <f>AVERAGE(B64:G64)</f>
+        <f t="shared" si="11"/>
         <v>13.989833333333335</v>
       </c>
       <c r="I64" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.14383333333333503</v>
       </c>
       <c r="J64" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.7833333333334949E-2</v>
       </c>
       <c r="K64" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.24016666666666531</v>
       </c>
       <c r="L64" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.43183333333333529</v>
       </c>
       <c r="M64" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.8166666666665137E-2</v>
       </c>
       <c r="N64" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.33516666666666417</v>
       </c>
     </row>
@@ -10025,31 +10058,31 @@
         <v>14.613</v>
       </c>
       <c r="H65" s="3">
-        <f>AVERAGE(B65:G65)</f>
+        <f t="shared" si="11"/>
         <v>14.245666666666667</v>
       </c>
       <c r="I65" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.11166666666666636</v>
       </c>
       <c r="J65" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5666666666666273E-2</v>
       </c>
       <c r="K65" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.17533333333333267</v>
       </c>
       <c r="L65" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.39966666666666661</v>
       </c>
       <c r="M65" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.5666666666666273E-2</v>
       </c>
       <c r="N65" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.36733333333333285</v>
       </c>
     </row>
@@ -10076,31 +10109,31 @@
         <v>14.804</v>
       </c>
       <c r="H66" s="3">
-        <f>AVERAGE(B66:G66)</f>
+        <f t="shared" ref="H66:H97" si="12">AVERAGE(B66:G66)</f>
         <v>14.468999999999999</v>
       </c>
       <c r="I66" s="3">
-        <f t="shared" si="0"/>
-        <v>4.8000000000000043E-2</v>
-      </c>
-      <c r="J66" s="3">
         <f t="shared" si="1"/>
         <v>4.8000000000000043E-2</v>
       </c>
+      <c r="J66" s="3">
+        <f t="shared" si="2"/>
+        <v>4.8000000000000043E-2</v>
+      </c>
       <c r="K66" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.14400000000000013</v>
       </c>
       <c r="L66" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.43099999999999916</v>
       </c>
       <c r="M66" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.8000000000000043E-2</v>
       </c>
       <c r="N66" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.33500000000000085</v>
       </c>
     </row>
@@ -10127,31 +10160,31 @@
         <v>14.996</v>
       </c>
       <c r="H67" s="3">
-        <f t="shared" ref="H67:H74" si="10">AVERAGE(B67:G67)</f>
+        <f t="shared" ref="H67:H74" si="13">AVERAGE(B67:G67)</f>
         <v>14.676666666666668</v>
       </c>
       <c r="I67" s="3">
-        <f t="shared" ref="I67:I74" si="11">H67-B67</f>
+        <f t="shared" ref="I67:I73" si="14">H67-B67</f>
         <v>6.3666666666668092E-2</v>
       </c>
       <c r="J67" s="3">
-        <f t="shared" ref="J67:J74" si="12">H67-C67</f>
+        <f t="shared" ref="J67:J74" si="15">H67-C67</f>
         <v>6.3666666666668092E-2</v>
       </c>
       <c r="K67" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.12733333333333263</v>
       </c>
       <c r="L67" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.35166666666666835</v>
       </c>
       <c r="M67" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-3.2333333333331993E-2</v>
       </c>
       <c r="N67" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.3193333333333328</v>
       </c>
     </row>
@@ -10178,31 +10211,31 @@
         <v>15.186999999999999</v>
       </c>
       <c r="H68" s="3">
+        <f t="shared" si="13"/>
+        <v>14.915999999999999</v>
+      </c>
+      <c r="I68" s="3">
+        <f t="shared" si="14"/>
+        <v>1.5999999999998238E-2</v>
+      </c>
+      <c r="J68" s="3">
+        <f t="shared" si="15"/>
+        <v>1.5999999999998238E-2</v>
+      </c>
+      <c r="K68" s="3">
+        <f t="shared" si="7"/>
+        <v>-8.0000000000001847E-2</v>
+      </c>
+      <c r="L68" s="3">
+        <f t="shared" si="8"/>
+        <v>0.39899999999999913</v>
+      </c>
+      <c r="M68" s="3">
+        <f t="shared" si="9"/>
+        <v>-8.0000000000001847E-2</v>
+      </c>
+      <c r="N68" s="3">
         <f t="shared" si="10"/>
-        <v>14.915999999999999</v>
-      </c>
-      <c r="I68" s="3">
-        <f t="shared" si="11"/>
-        <v>1.5999999999998238E-2</v>
-      </c>
-      <c r="J68" s="3">
-        <f t="shared" si="12"/>
-        <v>1.5999999999998238E-2</v>
-      </c>
-      <c r="K68" s="3">
-        <f t="shared" si="6"/>
-        <v>-8.0000000000001847E-2</v>
-      </c>
-      <c r="L68" s="3">
-        <f t="shared" si="7"/>
-        <v>0.39899999999999913</v>
-      </c>
-      <c r="M68" s="3">
-        <f t="shared" si="8"/>
-        <v>-8.0000000000001847E-2</v>
-      </c>
-      <c r="N68" s="3">
-        <f t="shared" si="9"/>
         <v>-0.2710000000000008</v>
       </c>
     </row>
@@ -10229,31 +10262,31 @@
         <v>15.473000000000001</v>
       </c>
       <c r="H69" s="3">
+        <f t="shared" si="13"/>
+        <v>15.170499999999999</v>
+      </c>
+      <c r="I69" s="3">
+        <f t="shared" si="14"/>
+        <v>7.949999999999946E-2</v>
+      </c>
+      <c r="J69" s="3">
+        <f t="shared" si="15"/>
+        <v>7.949999999999946E-2</v>
+      </c>
+      <c r="K69" s="3">
+        <f t="shared" si="7"/>
+        <v>-0.11150000000000126</v>
+      </c>
+      <c r="L69" s="3">
+        <f t="shared" si="8"/>
+        <v>0.36649999999999849</v>
+      </c>
+      <c r="M69" s="3">
+        <f t="shared" si="9"/>
+        <v>-0.11150000000000126</v>
+      </c>
+      <c r="N69" s="3">
         <f t="shared" si="10"/>
-        <v>15.170499999999999</v>
-      </c>
-      <c r="I69" s="3">
-        <f t="shared" si="11"/>
-        <v>7.949999999999946E-2</v>
-      </c>
-      <c r="J69" s="3">
-        <f t="shared" si="12"/>
-        <v>7.949999999999946E-2</v>
-      </c>
-      <c r="K69" s="3">
-        <f t="shared" si="6"/>
-        <v>-0.11150000000000126</v>
-      </c>
-      <c r="L69" s="3">
-        <f t="shared" si="7"/>
-        <v>0.36649999999999849</v>
-      </c>
-      <c r="M69" s="3">
-        <f t="shared" si="8"/>
-        <v>-0.11150000000000126</v>
-      </c>
-      <c r="N69" s="3">
-        <f t="shared" si="9"/>
         <v>-0.30250000000000199</v>
       </c>
     </row>
@@ -10280,31 +10313,31 @@
         <v>15.855</v>
       </c>
       <c r="H70" s="3">
+        <f t="shared" si="13"/>
+        <v>15.489166666666668</v>
+      </c>
+      <c r="I70" s="3">
+        <f t="shared" si="14"/>
+        <v>0.11116666666666752</v>
+      </c>
+      <c r="J70" s="3">
+        <f t="shared" si="15"/>
+        <v>0.11116666666666752</v>
+      </c>
+      <c r="K70" s="3">
+        <f t="shared" si="7"/>
+        <v>-0.17483333333333206</v>
+      </c>
+      <c r="L70" s="3">
+        <f t="shared" si="8"/>
+        <v>0.39816666666666833</v>
+      </c>
+      <c r="M70" s="3">
+        <f t="shared" si="9"/>
+        <v>-7.9833333333333201E-2</v>
+      </c>
+      <c r="N70" s="3">
         <f t="shared" si="10"/>
-        <v>15.489166666666668</v>
-      </c>
-      <c r="I70" s="3">
-        <f t="shared" si="11"/>
-        <v>0.11116666666666752</v>
-      </c>
-      <c r="J70" s="3">
-        <f t="shared" si="12"/>
-        <v>0.11116666666666752</v>
-      </c>
-      <c r="K70" s="3">
-        <f t="shared" si="6"/>
-        <v>-0.17483333333333206</v>
-      </c>
-      <c r="L70" s="3">
-        <f t="shared" si="7"/>
-        <v>0.39816666666666833</v>
-      </c>
-      <c r="M70" s="3">
-        <f t="shared" si="8"/>
-        <v>-7.9833333333333201E-2</v>
-      </c>
-      <c r="N70" s="3">
-        <f t="shared" si="9"/>
         <v>-0.36583333333333279</v>
       </c>
     </row>
@@ -10331,31 +10364,31 @@
         <v>15.951000000000001</v>
       </c>
       <c r="H71" s="3">
+        <f t="shared" si="13"/>
+        <v>15.616333333333335</v>
+      </c>
+      <c r="I71" s="3">
+        <f t="shared" si="14"/>
+        <v>-4.7666666666664526E-2</v>
+      </c>
+      <c r="J71" s="3">
+        <f t="shared" si="15"/>
+        <v>0.14333333333333442</v>
+      </c>
+      <c r="K71" s="3">
+        <f t="shared" si="7"/>
+        <v>-4.7666666666664526E-2</v>
+      </c>
+      <c r="L71" s="3">
+        <f t="shared" si="8"/>
+        <v>0.33433333333333515</v>
+      </c>
+      <c r="M71" s="3">
+        <f t="shared" si="9"/>
+        <v>-4.7666666666664526E-2</v>
+      </c>
+      <c r="N71" s="3">
         <f t="shared" si="10"/>
-        <v>15.616333333333335</v>
-      </c>
-      <c r="I71" s="3">
-        <f t="shared" si="11"/>
-        <v>-4.7666666666664526E-2</v>
-      </c>
-      <c r="J71" s="3">
-        <f t="shared" si="12"/>
-        <v>0.14333333333333442</v>
-      </c>
-      <c r="K71" s="3">
-        <f t="shared" si="6"/>
-        <v>-4.7666666666664526E-2</v>
-      </c>
-      <c r="L71" s="3">
-        <f t="shared" si="7"/>
-        <v>0.33433333333333515</v>
-      </c>
-      <c r="M71" s="3">
-        <f t="shared" si="8"/>
-        <v>-4.7666666666664526E-2</v>
-      </c>
-      <c r="N71" s="3">
-        <f t="shared" si="9"/>
         <v>-0.33466666666666534</v>
       </c>
     </row>
@@ -10382,31 +10415,31 @@
         <v>15.378</v>
       </c>
       <c r="H72" s="3">
+        <f t="shared" si="13"/>
+        <v>15.186833333333333</v>
+      </c>
+      <c r="I72" s="3">
+        <f t="shared" si="14"/>
+        <v>-1.6666666666687036E-4</v>
+      </c>
+      <c r="J72" s="3">
+        <f t="shared" si="15"/>
+        <v>-1.6666666666687036E-4</v>
+      </c>
+      <c r="K72" s="3">
+        <f t="shared" si="7"/>
+        <v>-9.516666666666751E-2</v>
+      </c>
+      <c r="L72" s="3">
+        <f t="shared" si="8"/>
+        <v>0.28683333333333216</v>
+      </c>
+      <c r="M72" s="3">
+        <f t="shared" si="9"/>
+        <v>-1.6666666666687036E-4</v>
+      </c>
+      <c r="N72" s="3">
         <f t="shared" si="10"/>
-        <v>15.186833333333333</v>
-      </c>
-      <c r="I72" s="3">
-        <f t="shared" si="11"/>
-        <v>-1.6666666666687036E-4</v>
-      </c>
-      <c r="J72" s="3">
-        <f t="shared" si="12"/>
-        <v>-1.6666666666687036E-4</v>
-      </c>
-      <c r="K72" s="3">
-        <f t="shared" si="6"/>
-        <v>-9.516666666666751E-2</v>
-      </c>
-      <c r="L72" s="3">
-        <f t="shared" si="7"/>
-        <v>0.28683333333333216</v>
-      </c>
-      <c r="M72" s="3">
-        <f t="shared" si="8"/>
-        <v>-1.6666666666687036E-4</v>
-      </c>
-      <c r="N72" s="3">
-        <f t="shared" si="9"/>
         <v>-0.1911666666666676</v>
       </c>
     </row>
@@ -10433,31 +10466,31 @@
         <v>15.090999999999999</v>
       </c>
       <c r="H73" s="3">
+        <f t="shared" si="13"/>
+        <v>15.027333333333331</v>
+      </c>
+      <c r="I73" s="3">
+        <f t="shared" si="14"/>
+        <v>-6.3666666666668092E-2</v>
+      </c>
+      <c r="J73" s="3">
+        <f t="shared" si="15"/>
+        <v>3.1333333333330771E-2</v>
+      </c>
+      <c r="K73" s="3">
+        <f t="shared" si="7"/>
+        <v>-6.3666666666668092E-2</v>
+      </c>
+      <c r="L73" s="3">
+        <f t="shared" si="8"/>
+        <v>0.22333333333333094</v>
+      </c>
+      <c r="M73" s="3">
+        <f t="shared" si="9"/>
+        <v>-6.3666666666668092E-2</v>
+      </c>
+      <c r="N73" s="3">
         <f t="shared" si="10"/>
-        <v>15.027333333333331</v>
-      </c>
-      <c r="I73" s="3">
-        <f t="shared" si="11"/>
-        <v>-6.3666666666668092E-2</v>
-      </c>
-      <c r="J73" s="3">
-        <f t="shared" si="12"/>
-        <v>3.1333333333330771E-2</v>
-      </c>
-      <c r="K73" s="3">
-        <f t="shared" si="6"/>
-        <v>-6.3666666666668092E-2</v>
-      </c>
-      <c r="L73" s="3">
-        <f t="shared" si="7"/>
-        <v>0.22333333333333094</v>
-      </c>
-      <c r="M73" s="3">
-        <f t="shared" si="8"/>
-        <v>-6.3666666666668092E-2</v>
-      </c>
-      <c r="N73" s="3">
-        <f t="shared" si="9"/>
         <v>-6.3666666666668092E-2</v>
       </c>
     </row>
@@ -10481,28 +10514,28 @@
         <v>15.186999999999999</v>
       </c>
       <c r="H74" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>15.206</v>
       </c>
       <c r="I74" s="3"/>
       <c r="J74" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>-0.1720000000000006</v>
       </c>
       <c r="K74" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.9000000000000128E-2</v>
       </c>
       <c r="L74" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.30599999999999916</v>
       </c>
       <c r="M74" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.1720000000000006</v>
       </c>
       <c r="N74" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.9000000000000128E-2</v>
       </c>
     </row>
@@ -10578,19 +10611,19 @@
         <v>-7.4895833333333106E-2</v>
       </c>
       <c r="J78" s="3">
-        <f t="shared" ref="J78:N78" si="13">AVERAGE(J2:J74)</f>
+        <f t="shared" ref="J78:M78" si="16">AVERAGE(J2:J74)</f>
         <v>-3.459589041095875E-2</v>
       </c>
       <c r="K78" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>4.5547945205478904E-3</v>
       </c>
       <c r="L78" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.18869178082191784</v>
       </c>
       <c r="M78" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>5.0678082191780729E-2</v>
       </c>
       <c r="N78" s="3">

</xml_diff>